<commit_message>
"updated http response code in validation rules"
</commit_message>
<xml_diff>
--- a/data-items/Employer_Submission_RPN_Validation_Rules.xlsx
+++ b/data-items/Employer_Submission_RPN_Validation_Rules.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="253">
   <si>
     <t>Payslip</t>
   </si>
@@ -22402,8 +22402,8 @@
   <dimension ref="A1:BN453"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105:O105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -23400,7 +23400,7 @@
       <c r="G16" s="68">
         <v>400</v>
       </c>
-      <c r="H16" s="62" t="s">
+      <c r="H16" s="24" t="s">
         <v>242</v>
       </c>
       <c r="I16" s="62" t="s">
@@ -23447,7 +23447,7 @@
       <c r="G17" s="62">
         <v>400</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="H17" s="24" t="s">
         <v>242</v>
       </c>
       <c r="I17" s="62" t="s">
@@ -23494,7 +23494,7 @@
       <c r="G18" s="62">
         <v>400</v>
       </c>
-      <c r="H18" s="62" t="s">
+      <c r="H18" s="24" t="s">
         <v>242</v>
       </c>
       <c r="I18" s="62" t="s">
@@ -23539,7 +23539,7 @@
         <v>156</v>
       </c>
       <c r="G19" s="55">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H19" s="55" t="s">
         <v>243</v>
@@ -23586,7 +23586,7 @@
         <v>156</v>
       </c>
       <c r="G20" s="55">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H20" s="55" t="s">
         <v>243</v>
@@ -23847,8 +23847,8 @@
       <c r="F24" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G24" s="45" t="s">
-        <v>12</v>
+      <c r="G24" s="24">
+        <v>200</v>
       </c>
       <c r="H24" s="24" t="s">
         <v>243</v>
@@ -23941,8 +23941,8 @@
       <c r="F26" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G26" s="45" t="s">
-        <v>12</v>
+      <c r="G26" s="24">
+        <v>200</v>
       </c>
       <c r="H26" s="55" t="s">
         <v>243</v>
@@ -23988,8 +23988,8 @@
       <c r="F27" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G27" s="45" t="s">
-        <v>12</v>
+      <c r="G27" s="24">
+        <v>200</v>
       </c>
       <c r="H27" s="55" t="s">
         <v>243</v>
@@ -24035,8 +24035,8 @@
       <c r="F28" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G28" s="45" t="s">
-        <v>12</v>
+      <c r="G28" s="24">
+        <v>200</v>
       </c>
       <c r="H28" s="55" t="s">
         <v>243</v>
@@ -24082,8 +24082,8 @@
       <c r="F29" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G29" s="45" t="s">
-        <v>12</v>
+      <c r="G29" s="24">
+        <v>200</v>
       </c>
       <c r="H29" s="55" t="s">
         <v>243</v>
@@ -24129,8 +24129,8 @@
       <c r="F30" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G30" s="45" t="s">
-        <v>12</v>
+      <c r="G30" s="24">
+        <v>200</v>
       </c>
       <c r="H30" s="24" t="s">
         <v>243</v>
@@ -24176,8 +24176,8 @@
       <c r="F31" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="G31" s="68" t="s">
-        <v>12</v>
+      <c r="G31" s="24">
+        <v>200</v>
       </c>
       <c r="H31" s="62" t="s">
         <v>243</v>
@@ -24223,8 +24223,8 @@
       <c r="F32" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G32" s="45" t="s">
-        <v>12</v>
+      <c r="G32" s="24">
+        <v>200</v>
       </c>
       <c r="H32" s="24" t="s">
         <v>243</v>
@@ -24317,8 +24317,8 @@
       <c r="F34" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G34" s="45" t="s">
-        <v>12</v>
+      <c r="G34" s="24">
+        <v>200</v>
       </c>
       <c r="H34" s="24" t="s">
         <v>243</v>
@@ -24364,8 +24364,8 @@
       <c r="F35" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G35" s="24" t="s">
-        <v>12</v>
+      <c r="G35" s="24">
+        <v>200</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>243</v>
@@ -24411,8 +24411,8 @@
       <c r="F36" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G36" s="45" t="s">
-        <v>12</v>
+      <c r="G36" s="24">
+        <v>200</v>
       </c>
       <c r="H36" s="24" t="s">
         <v>243</v>
@@ -24458,8 +24458,8 @@
       <c r="F37" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G37" s="45" t="s">
-        <v>12</v>
+      <c r="G37" s="24">
+        <v>200</v>
       </c>
       <c r="H37" s="24" t="s">
         <v>243</v>
@@ -24603,8 +24603,8 @@
       <c r="F39" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G39" s="45" t="s">
-        <v>12</v>
+      <c r="G39" s="24">
+        <v>200</v>
       </c>
       <c r="H39" s="24" t="s">
         <v>243</v>
@@ -24650,8 +24650,8 @@
       <c r="F40" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G40" s="45" t="s">
-        <v>12</v>
+      <c r="G40" s="24">
+        <v>200</v>
       </c>
       <c r="H40" s="24" t="s">
         <v>243</v>
@@ -24748,8 +24748,8 @@
       <c r="F41" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G41" s="45" t="s">
-        <v>12</v>
+      <c r="G41" s="24">
+        <v>200</v>
       </c>
       <c r="H41" s="24" t="s">
         <v>243</v>
@@ -24846,8 +24846,8 @@
       <c r="F42" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G42" s="45" t="s">
-        <v>12</v>
+      <c r="G42" s="24">
+        <v>200</v>
       </c>
       <c r="H42" s="24" t="s">
         <v>243</v>
@@ -24893,8 +24893,8 @@
       <c r="F43" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G43" s="45" t="s">
-        <v>12</v>
+      <c r="G43" s="24">
+        <v>200</v>
       </c>
       <c r="H43" s="24" t="s">
         <v>243</v>
@@ -24940,8 +24940,8 @@
       <c r="F44" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G44" s="45" t="s">
-        <v>12</v>
+      <c r="G44" s="24">
+        <v>200</v>
       </c>
       <c r="H44" s="24" t="s">
         <v>243</v>
@@ -24987,8 +24987,8 @@
       <c r="F45" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G45" s="45" t="s">
-        <v>12</v>
+      <c r="G45" s="24">
+        <v>200</v>
       </c>
       <c r="H45" s="24" t="s">
         <v>243</v>
@@ -25034,8 +25034,8 @@
       <c r="F46" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G46" s="45" t="s">
-        <v>12</v>
+      <c r="G46" s="24">
+        <v>200</v>
       </c>
       <c r="H46" s="24" t="s">
         <v>243</v>
@@ -25128,8 +25128,8 @@
       <c r="F48" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G48" s="45" t="s">
-        <v>12</v>
+      <c r="G48" s="24">
+        <v>200</v>
       </c>
       <c r="H48" s="24" t="s">
         <v>243</v>
@@ -25226,8 +25226,8 @@
       <c r="F49" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G49" s="45" t="s">
-        <v>12</v>
+      <c r="G49" s="24">
+        <v>200</v>
       </c>
       <c r="H49" s="24" t="s">
         <v>243</v>
@@ -25273,8 +25273,8 @@
       <c r="F50" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G50" s="45" t="s">
-        <v>12</v>
+      <c r="G50" s="24">
+        <v>200</v>
       </c>
       <c r="H50" s="24" t="s">
         <v>243</v>
@@ -25320,8 +25320,8 @@
       <c r="F51" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G51" s="45" t="s">
-        <v>12</v>
+      <c r="G51" s="24">
+        <v>200</v>
       </c>
       <c r="H51" s="24" t="s">
         <v>243</v>
@@ -25367,8 +25367,8 @@
       <c r="F52" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G52" s="45" t="s">
-        <v>12</v>
+      <c r="G52" s="24">
+        <v>200</v>
       </c>
       <c r="H52" s="24" t="s">
         <v>243</v>
@@ -25395,7 +25395,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:66" s="81" customFormat="1" ht="43.2" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:66" s="81" customFormat="1" ht="46.8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A53" s="62">
         <v>49</v>
       </c>
@@ -25414,14 +25414,14 @@
       <c r="F53" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="G53" s="62" t="s">
-        <v>12</v>
+      <c r="G53" s="24">
+        <v>200</v>
       </c>
       <c r="H53" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="I53" s="62" t="s">
-        <v>245</v>
+      <c r="I53" s="24" t="s">
+        <v>246</v>
       </c>
       <c r="J53" s="62" t="s">
         <v>7</v>
@@ -25461,8 +25461,8 @@
       <c r="F54" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G54" s="45" t="s">
-        <v>12</v>
+      <c r="G54" s="24">
+        <v>200</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>243</v>
@@ -25559,8 +25559,8 @@
       <c r="F55" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G55" s="45" t="s">
-        <v>12</v>
+      <c r="G55" s="24">
+        <v>200</v>
       </c>
       <c r="H55" s="24" t="s">
         <v>243</v>
@@ -25658,7 +25658,7 @@
         <v>156</v>
       </c>
       <c r="G56" s="55">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H56" s="24" t="s">
         <v>243</v>
@@ -37627,21 +37627,21 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="15">
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A57:O57"/>
+    <mergeCell ref="A70:O70"/>
+    <mergeCell ref="A84:O84"/>
+    <mergeCell ref="A83:O83"/>
+    <mergeCell ref="A105:O105"/>
+    <mergeCell ref="A71:O71"/>
+    <mergeCell ref="A58:O58"/>
     <mergeCell ref="A125:O125"/>
     <mergeCell ref="A126:O126"/>
     <mergeCell ref="A119:O119"/>
     <mergeCell ref="A103:O103"/>
     <mergeCell ref="A106:O106"/>
-    <mergeCell ref="A84:O84"/>
-    <mergeCell ref="A83:O83"/>
-    <mergeCell ref="A105:O105"/>
-    <mergeCell ref="A71:O71"/>
-    <mergeCell ref="A58:O58"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="A57:O57"/>
-    <mergeCell ref="A70:O70"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J65:J69 J49:J55 J114:J118 J78:J82 J104 J120:J124 J7:J8 J62:J63 J75:J76 J88:J90 J110:J112 J130:J131 J10:J16 J133:J145 J92:J102 J21:J22 J24:J47">

</xml_diff>